<commit_message>
added more antibiotics and rules
</commit_message>
<xml_diff>
--- a/antibiotics.xlsx
+++ b/antibiotics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Code/CDSS Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10A9885-D3D2-8A4C-99CC-CC03ADB4BA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E563AD0-B72B-D440-BF10-9760E09D22DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="9020" windowWidth="26440" windowHeight="15360" xr2:uid="{CEA8BBAA-D33C-6043-B829-CECE4A5E67DC}"/>
+    <workbookView xWindow="1940" yWindow="4080" windowWidth="26440" windowHeight="15360" xr2:uid="{CEA8BBAA-D33C-6043-B829-CECE4A5E67DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="70">
   <si>
     <t>advice</t>
   </si>
@@ -61,9 +61,6 @@
     <t>BID</t>
   </si>
   <si>
-    <t xml:space="preserve">Questionable succes when used in abscesses (especially Strep. Zooepidemicus). High concentration in the urine, penetrates the blood-brain-barrier. </t>
-  </si>
-  <si>
     <t>Chloramphenicol</t>
   </si>
   <si>
@@ -145,20 +142,125 @@
     <t>Aminoglykoside</t>
   </si>
   <si>
+    <t>7 mg/kg</t>
+  </si>
+  <si>
     <t>Does not work in abscesses or in anaerobic milieu. In Foals &lt;1 month, use Amikacin instead.</t>
   </si>
   <si>
     <t>7 mg/kg (Foals &lt;2 weeks: 12mg/kg)</t>
+  </si>
+  <si>
+    <t>Amikacin</t>
+  </si>
+  <si>
+    <t>30 mg/kg (Foals &lt; 1 week) / 20-25 mg/kg (Foals 2-4 weeks)</t>
+  </si>
+  <si>
+    <t>First line antibiotic in foals. Drug repurposing from human medicine. Does not work in abscesser or in anaerobic milieu.</t>
+  </si>
+  <si>
+    <t>Oxytetracyclin</t>
+  </si>
+  <si>
+    <t>Tetrazykline</t>
+  </si>
+  <si>
+    <t>Doxycyclin</t>
+  </si>
+  <si>
+    <t>10 mg/kg</t>
+  </si>
+  <si>
+    <t>Drug repurposing from human medicine, intracellular effect. Works against Ehrlichia, Rickettsia, Anaplasma. Does not penetrate the blood-brain-barrier; in general good tissue penetration. Careful use of Tetracyclines in growing patients.</t>
+  </si>
+  <si>
+    <t>Metronidazole</t>
+  </si>
+  <si>
+    <t>Nitroimidazole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not use in farm animals! Good as additional antibiotics when dealing with anaerobic bacteria. </t>
+  </si>
+  <si>
+    <t>15 mg/kg</t>
+  </si>
+  <si>
+    <t>Azithromycin</t>
+  </si>
+  <si>
+    <t>Macrolides</t>
+  </si>
+  <si>
+    <t>Clarithromycin</t>
+  </si>
+  <si>
+    <t>7.5 mg/kg</t>
+  </si>
+  <si>
+    <t>Rifampicin</t>
+  </si>
+  <si>
+    <t>Rifamycin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 mg/kg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">per os </t>
+  </si>
+  <si>
+    <t>Drug repurposing from human medicine, intracellular effect. Works well in abscesses. Can color urine orange. Use only in combination with other antibiotics.</t>
+  </si>
+  <si>
+    <t>Drug repurposing from human medicine. CAVE: danger of potential colitis in adult equines. First line AB in R.equi (in combination with Rifampicin). Works well in abscesses.</t>
+  </si>
+  <si>
+    <t>Cefquinom</t>
+  </si>
+  <si>
+    <t>4 mg/kg</t>
+  </si>
+  <si>
+    <t>SID (Foals BID)</t>
+  </si>
+  <si>
+    <t>1 mg/kg</t>
+  </si>
+  <si>
+    <t>Foals: 1 mg/kg as prophylaxis, 4.5 mg/kg as therapy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 mg/kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intramuscular </t>
+  </si>
+  <si>
+    <t>Ceftiofur</t>
+  </si>
+  <si>
+    <t>Drug repurposing from human medicine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Questionable success when used in abscesses (especially Strep. Zooepidemicus). High concentration in the urine, penetrates the blood-brain-barrier. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -515,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8BBC06-7AC3-4E44-AD54-C7BB467EC790}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,16 +637,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -553,7 +655,7 @@
         <v>2</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
@@ -564,13 +666,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
@@ -582,120 +684,471 @@
         <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="119" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="I4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>36</v>
       </c>
     </row>
+    <row r="7" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added info_texts, refactoring etc
</commit_message>
<xml_diff>
--- a/antibiotics.xlsx
+++ b/antibiotics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Code/CDSS Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E563AD0-B72B-D440-BF10-9760E09D22DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98568797-8CD2-E648-8D74-9E188A8C3201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="4080" windowWidth="26440" windowHeight="15360" xr2:uid="{CEA8BBAA-D33C-6043-B829-CECE4A5E67DC}"/>
+    <workbookView xWindow="3340" yWindow="1380" windowWidth="24460" windowHeight="15360" xr2:uid="{CEA8BBAA-D33C-6043-B829-CECE4A5E67DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="77">
   <si>
     <t>advice</t>
   </si>
@@ -245,6 +245,27 @@
   </si>
   <si>
     <t xml:space="preserve">Questionable success when used in abscesses (especially Strep. Zooepidemicus). High concentration in the urine, penetrates the blood-brain-barrier. </t>
+  </si>
+  <si>
+    <t>Fluorchinolone</t>
+  </si>
+  <si>
+    <t>SID / BID</t>
+  </si>
+  <si>
+    <t>Drug repurposing; intracellular activity. Works well in abscesses, reaches 25% concentration in central nervous system. Always dilute 1:1. Application BID for gram-positive or unknown bacteria; application SID for gram-negative bacteria. Careful use in foals.</t>
+  </si>
+  <si>
+    <t>Marbofloxacin</t>
+  </si>
+  <si>
+    <t>Enrofloxacin</t>
+  </si>
+  <si>
+    <t>2 mg/kg</t>
+  </si>
+  <si>
+    <t>3 mg/kg</t>
   </si>
 </sst>
 </file>
@@ -617,18 +638,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8BBC06-7AC3-4E44-AD54-C7BB467EC790}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="32.6640625" style="1" customWidth="1"/>
-    <col min="3" max="5" width="29.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="1" customWidth="1"/>
     <col min="6" max="8" width="10.83203125" style="1"/>
-    <col min="9" max="9" width="21.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="32" style="1" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1147,6 +1170,110 @@
         <v>68</v>
       </c>
     </row>
+    <row r="20" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="136" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added all rules/antibiotics (except eye)
</commit_message>
<xml_diff>
--- a/antibiotics.xlsx
+++ b/antibiotics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Code/CDSS Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98568797-8CD2-E648-8D74-9E188A8C3201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9D8ED4-A03F-D94E-BBF3-AC329D055E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3340" yWindow="1380" windowWidth="24460" windowHeight="15360" xr2:uid="{CEA8BBAA-D33C-6043-B829-CECE4A5E67DC}"/>
   </bookViews>
@@ -133,9 +133,6 @@
     <t>SID</t>
   </si>
   <si>
-    <t>Bad penetration into the central nervous system and abscesses. Commonly administered in combination with Gentamicin.</t>
-  </si>
-  <si>
     <t>Gentamicin</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t>7 mg/kg</t>
   </si>
   <si>
-    <t>Does not work in abscesses or in anaerobic milieu. In Foals &lt;1 month, use Amikacin instead.</t>
-  </si>
-  <si>
     <t>7 mg/kg (Foals &lt;2 weeks: 12mg/kg)</t>
   </si>
   <si>
@@ -157,9 +151,6 @@
     <t>30 mg/kg (Foals &lt; 1 week) / 20-25 mg/kg (Foals 2-4 weeks)</t>
   </si>
   <si>
-    <t>First line antibiotic in foals. Drug repurposing from human medicine. Does not work in abscesser or in anaerobic milieu.</t>
-  </si>
-  <si>
     <t>Oxytetracyclin</t>
   </si>
   <si>
@@ -172,9 +163,6 @@
     <t>10 mg/kg</t>
   </si>
   <si>
-    <t>Drug repurposing from human medicine, intracellular effect. Works against Ehrlichia, Rickettsia, Anaplasma. Does not penetrate the blood-brain-barrier; in general good tissue penetration. Careful use of Tetracyclines in growing patients.</t>
-  </si>
-  <si>
     <t>Metronidazole</t>
   </si>
   <si>
@@ -241,9 +229,6 @@
     <t>Ceftiofur</t>
   </si>
   <si>
-    <t>Drug repurposing from human medicine.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Questionable success when used in abscesses (especially Strep. Zooepidemicus). High concentration in the urine, penetrates the blood-brain-barrier. </t>
   </si>
   <si>
@@ -266,6 +251,21 @@
   </si>
   <si>
     <t>3 mg/kg</t>
+  </si>
+  <si>
+    <t>Bad penetration into the central nervous system and abscesses. Commonly administered in combination with Gentamicin. Do not mix Penicillin and Aminoglykosides (Gentamicin/Amikacin) in one syringe.</t>
+  </si>
+  <si>
+    <t>Does not work in abscesses or in anaerobic milieu. In Foals &lt;1 month, use Amikacin instead. Do not mix Penicillin and Aminoglykosides (Gentamicin/Amikacin) in one syringe.</t>
+  </si>
+  <si>
+    <t>First line antibiotic in foals. Drug repurposing from human medicine. Does not work in abscesses or in anaerobic milieu. Do not mix Penicillin and Aminoglykosides (Gentamicin/Amikacin) in one syringe.</t>
+  </si>
+  <si>
+    <t>Drug repurposing from veterinary medicine, intracellular effect. Works against Ehrlichia, Rickettsia, Anaplasma. Does not penetrate the blood-brain-barrier; in general good tissue penetration. Careful use of Tetracyclines in growing patients.</t>
+  </si>
+  <si>
+    <t>Drug repurposing from veterinary medicine.</t>
   </si>
 </sst>
 </file>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8BBC06-7AC3-4E44-AD54-C7BB467EC790}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="101" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="102" x14ac:dyDescent="0.2">
@@ -736,7 +736,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -762,7 +762,7 @@
         <v>26</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -794,12 +794,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>23</v>
@@ -808,7 +808,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>25</v>
@@ -817,15 +817,15 @@
         <v>31</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>10</v>
@@ -834,7 +834,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>25</v>
@@ -843,15 +843,15 @@
         <v>31</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="119" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
@@ -863,7 +863,7 @@
         <v>23</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>25</v>
@@ -872,15 +872,15 @@
         <v>7</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
@@ -892,7 +892,7 @@
         <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>6</v>
@@ -901,15 +901,15 @@
         <v>7</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
@@ -924,21 +924,21 @@
         <v>7</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>25</v>
@@ -947,15 +947,15 @@
         <v>7</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>11</v>
@@ -967,7 +967,7 @@
         <v>23</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>6</v>
@@ -976,15 +976,15 @@
         <v>31</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>11</v>
@@ -996,7 +996,7 @@
         <v>23</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>6</v>
@@ -1005,15 +1005,15 @@
         <v>7</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>11</v>
@@ -1025,24 +1025,24 @@
         <v>10</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>11</v>
@@ -1054,21 +1054,21 @@
         <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>31</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>22</v>
@@ -1080,21 +1080,21 @@
         <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>22</v>
@@ -1106,21 +1106,21 @@
         <v>10</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>22</v>
@@ -1132,7 +1132,7 @@
         <v>10</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>25</v>
@@ -1141,12 +1141,12 @@
         <v>7</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
@@ -1158,7 +1158,7 @@
         <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>30</v>
@@ -1167,15 +1167,15 @@
         <v>7</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
@@ -1184,24 +1184,24 @@
         <v>11</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>23</v>
@@ -1210,50 +1210,50 @@
         <v>11</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="136" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>10</v>
@@ -1262,16 +1262,16 @@
         <v>10</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed double boxes for different dosages
</commit_message>
<xml_diff>
--- a/antibiotics.xlsx
+++ b/antibiotics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bboen\Documents\Repositories\CDSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FE695C-2E77-4196-A3C8-3AB8742D4459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878A8794-FEAF-4A22-979D-63E86C3A3BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="109380" yWindow="7680" windowWidth="29625" windowHeight="16125" xr2:uid="{CEA8BBAA-D33C-6043-B829-CECE4A5E67DC}"/>
+    <workbookView xWindow="100680" yWindow="3180" windowWidth="38640" windowHeight="21120" xr2:uid="{CEA8BBAA-D33C-6043-B829-CECE4A5E67DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="79">
   <si>
     <t>advice</t>
   </si>
@@ -644,24 +644,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8BBC06-7AC3-4E44-AD54-C7BB467EC790}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="101" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="2" width="32.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="32.6875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1875" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="1" customWidth="1"/>
-    <col min="6" max="8" width="10.83203125" style="1"/>
+    <col min="6" max="8" width="10.8125" style="1"/>
     <col min="9" max="9" width="32" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="16384" width="10.8125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -690,7 +690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="78.75" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -716,7 +716,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="78.75" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -745,7 +745,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="62" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="63" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>69</v>
       </c>
@@ -774,7 +774,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>70</v>
       </c>
@@ -803,7 +803,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="62" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="63" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -829,7 +829,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="93" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="94.5" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -855,7 +855,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="110.25" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
@@ -884,7 +884,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="110.25" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>65</v>
       </c>
@@ -913,7 +913,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -936,7 +936,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="47.25" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -959,7 +959,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="93" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="94.5" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -988,7 +988,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="110.25" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="78.75" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -1046,36 +1046,33 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
@@ -1089,10 +1086,10 @@
         <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>47</v>
@@ -1101,9 +1098,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>19</v>
@@ -1115,19 +1112,19 @@
         <v>9</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
@@ -1144,7 +1141,7 @@
         <v>46</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>6</v>
@@ -1153,33 +1150,33 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="126" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="124" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="126" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>56</v>
       </c>
@@ -1193,10 +1190,10 @@
         <v>10</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>53</v>
@@ -1205,24 +1202,24 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="124" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="126" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>53</v>
@@ -1231,7 +1228,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="124" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="126" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
@@ -1245,41 +1242,15 @@
         <v>9</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>53</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="124" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" s="1" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>